<commit_message>
add 3 possible basin names
</commit_message>
<xml_diff>
--- a/inst/extdata/Address_table.xlsx
+++ b/inst/extdata/Address_table.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Rprojects\AllWaterThai\inst\extdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4470C8A6-19D0-4467-B2DD-1677DEC85C6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA92F9EC-60E1-4CF1-B832-49304C7ED0BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{C7D1CF2D-BB7E-4D2C-B4B4-F3A544ABF6EE}"/>
+    <workbookView xWindow="4605" yWindow="930" windowWidth="15015" windowHeight="11655" xr2:uid="{C7D1CF2D-BB7E-4D2C-B4B4-F3A544ABF6EE}"/>
   </bookViews>
   <sheets>
     <sheet name="MB_AREA_ALL" sheetId="4" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">MB_AREA_ALL!$A$1:$C$21</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">MB_AREA_ALL!$A$1:$C$20</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="55">
   <si>
     <t>เกาะยอ</t>
   </si>
@@ -48,9 +48,6 @@
     <t>โคกสลุง</t>
   </si>
   <si>
-    <t>วังทอง</t>
-  </si>
-  <si>
     <t>ชัยนาท</t>
   </si>
   <si>
@@ -78,9 +75,6 @@
     <t>ด่านขุนทด</t>
   </si>
   <si>
-    <t>วังเหนือ</t>
-  </si>
-  <si>
     <t>เวียงเหนือ</t>
   </si>
   <si>
@@ -166,9 +160,6 @@
   </si>
   <si>
     <t>นครราชสีมา</t>
-  </si>
-  <si>
-    <t>ลำปาง</t>
   </si>
   <si>
     <t>พะเยา</t>
@@ -254,7 +245,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -268,9 +259,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -587,10 +575,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25DFFE09-76BA-432A-A857-C8C047E06800}">
-  <dimension ref="A1:F21"/>
+  <dimension ref="A1:F20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="21"/>
@@ -605,236 +593,225 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" s="5" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="D1" s="3"/>
       <c r="E1" s="3"/>
       <c r="F1" s="1"/>
     </row>
     <row r="2" spans="1:6">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="6" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="6" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
-      <c r="A3" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" s="7" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6">
-      <c r="A4" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" s="7" t="s">
+    <row r="7" spans="1:6">
+      <c r="A7" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="C11" s="6" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
-      <c r="A5" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B5" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="C5" s="7" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6">
-      <c r="A6" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="B6" s="7" t="s">
+    <row r="12" spans="1:6">
+      <c r="A12" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="C6" s="7" t="s">
+      <c r="B12" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="C12" s="6" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
-      <c r="A7" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="B7" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="C7" s="7" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6">
-      <c r="A8" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="B8" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="C8" s="7" t="s">
+    <row r="13" spans="1:6">
+      <c r="A13" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="B16" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B18" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="C18" s="6" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
-      <c r="A9" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="B9" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="C9" s="7" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6">
-      <c r="A10" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="B10" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="C10" s="7" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6">
-      <c r="A11" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="B11" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="C11" s="7" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6">
-      <c r="A12" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="B12" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="C12" s="7" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6">
-      <c r="A13" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="B13" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="C13" s="7" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6">
-      <c r="A14" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="B14" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="C14" s="7" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6">
-      <c r="A15" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="B15" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="C15" s="7" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6">
-      <c r="A16" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="B16" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="C16" s="7" t="s">
+    <row r="19" spans="1:3">
+      <c r="A19" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B19" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="C19" s="6" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="17" spans="1:3">
-      <c r="A17" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="B17" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="C17" s="7" t="s">
+    <row r="20" spans="1:3">
+      <c r="A20" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="B20" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C20" s="6" t="s">
         <v>51</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3">
-      <c r="A18" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="B18" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="C18" s="7" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3">
-      <c r="A19" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="B19" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="C19" s="7" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3">
-      <c r="A20" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="B20" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="C20" s="7" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3">
-      <c r="A21" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="B21" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="C21" s="7" t="s">
-        <v>54</v>
       </c>
     </row>
   </sheetData>

</xml_diff>